<commit_message>
update computation of inlet concentrations for ADM1-R3-frac based on lab analysis data from 2018-2020.
</commit_message>
<xml_diff>
--- a/Matlab/nfg-biosim-softsensor-backup/2021_Labordaten_landwirtschaftliche_Substrate.xlsx
+++ b/Matlab/nfg-biosim-softsensor-backup/2021_Labordaten_landwirtschaftliche_Substrate.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dbfz-user.leipzig.dbfz.de\user$\shellmann\Notizen &amp; Unterlagen\Messdaten\Labordaten 2021_2022 final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4110F3DF-BB02-4998-87DE-8A5A3DB302DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF3A16D-168E-4C3E-89AA-1B64205A659E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="5" xr2:uid="{AEE4862D-4A3E-49D3-987F-015B00AA3EF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" activeTab="5" xr2:uid="{AEE4862D-4A3E-49D3-987F-015B00AA3EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Maissilage" sheetId="1" r:id="rId1"/>
     <sheet name="Grassilage" sheetId="4" r:id="rId2"/>
     <sheet name="Getreidestroh" sheetId="7" r:id="rId3"/>
-    <sheet name="Rinderguelle" sheetId="3" r:id="rId4"/>
-    <sheet name="Schweineguelle" sheetId="5" r:id="rId5"/>
-    <sheet name="HTK" sheetId="6" r:id="rId6"/>
+    <sheet name="Zuckerruebensilage" sheetId="8" r:id="rId4"/>
+    <sheet name="Rinderguelle" sheetId="3" r:id="rId5"/>
+    <sheet name="Schweineguelle" sheetId="5" r:id="rId6"/>
+    <sheet name="HTK" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>Probeneingangsnummer</t>
   </si>
@@ -219,13 +220,25 @@
   </si>
   <si>
     <t>BK-21-1686</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>in Futtermittelübersicht steht BK-13-1381, in GC-Daten gibt’s aber nur BK-21-1381 mit sonst gleichen Attributen. Das muss es sein.</t>
+  </si>
+  <si>
+    <t>BK-21-0453</t>
+  </si>
+  <si>
+    <t>Rübenmus, aber sollte in etwa passen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +267,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,11 +320,110 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="42"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -623,28 +741,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A464897B-AA9E-468D-815C-0C802AF1F274}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,436 +796,442 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>29.16</v>
+        <v>33.82</v>
       </c>
       <c r="C2">
-        <v>70.84</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="D2">
-        <v>0.31169600000000003</v>
+        <v>0.26472000000000007</v>
       </c>
       <c r="E2">
-        <v>54.80000000000004</v>
+        <v>33.499999999999943</v>
       </c>
       <c r="F2">
-        <v>89.617581618104794</v>
+        <v>66.50553439145925</v>
       </c>
       <c r="G2">
-        <v>25.195391114113143</v>
+        <v>38.671351790487883</v>
       </c>
       <c r="H2">
         <f>1000-E2-F2-G2</f>
-        <v>830.38702726778206</v>
-      </c>
-      <c r="I2" s="8">
-        <v>91.623333333333335</v>
+        <v>861.32311381805289</v>
+      </c>
+      <c r="I2" s="9">
+        <v>130.92333333333332</v>
       </c>
       <c r="J2">
         <v>10</v>
       </c>
       <c r="K2" s="6">
         <f>I2*J2</f>
-        <v>916.23333333333335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1309.2333333333331</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>95.28</v>
+      </c>
+      <c r="C3">
+        <v>4.7199999999999989</v>
+      </c>
+      <c r="D3">
+        <v>5.8999999999999983E-2</v>
+      </c>
+      <c r="E3">
+        <v>35.499999999999972</v>
+      </c>
+      <c r="F3">
+        <v>71.926511192147345</v>
+      </c>
+      <c r="G3">
+        <v>34.250243788566472</v>
+      </c>
+      <c r="H3">
+        <f>1000-E3-F3-G3</f>
+        <v>858.32324501928622</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>29.16</v>
+      </c>
+      <c r="C4">
+        <v>70.84</v>
+      </c>
+      <c r="D4">
+        <v>0.31169600000000003</v>
+      </c>
+      <c r="E4">
+        <v>54.80000000000004</v>
+      </c>
+      <c r="F4">
+        <v>89.617581618104794</v>
+      </c>
+      <c r="G4">
+        <v>25.195391114113143</v>
+      </c>
+      <c r="H4">
+        <f>1000-E4-F4-G4</f>
+        <v>830.38702726778206</v>
+      </c>
+      <c r="I4" s="8">
+        <v>592.75999999999988</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="6">
+        <f>I4*J4</f>
+        <v>1185.5199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>35.76</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>64.240000000000009</v>
       </c>
-      <c r="D3">
+      <c r="D5">
         <v>0.45610400000000006</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>55.600000000000023</v>
       </c>
-      <c r="F3">
+      <c r="F5">
         <v>90.441729212797412</v>
       </c>
-      <c r="G3">
+      <c r="G5">
         <v>15.695100242413339</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H18" si="0">1000-E3-F3-G3</f>
+      <c r="H5">
+        <f>1000-E5-F5-G5</f>
         <v>838.2631705447892</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I5" s="8">
         <v>57.856666666666662</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K15" si="1">I3*J3</f>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6">
+        <f>I5*J5</f>
         <v>115.71333333333332</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>29.33</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>70.67</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>0.35335</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>48.199999999999932</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>90.553051231102117</v>
       </c>
-      <c r="G4">
+      <c r="G6">
         <v>27.941620424978012</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
+      <c r="H6">
+        <f>1000-E6-F6-G6</f>
         <v>833.30532834391988</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I6" s="8">
         <v>421.91333333333336</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" si="1"/>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6">
+        <f>I6*J6</f>
         <v>843.82666666666671</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>21.04</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>78.960000000000008</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <v>0.48165600000000003</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>90.19999999999996</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>117.86290335788468</v>
       </c>
-      <c r="G5">
+      <c r="G7">
         <v>36.048146525533241</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f>1000-E7-F7-G7</f>
         <v>755.88895011658224</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I7" s="8">
         <v>375.53999999999996</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="6">
-        <f t="shared" si="1"/>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6">
+        <f>I7*J7</f>
         <v>751.07999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>31.67</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>68.33</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>0.30065200000000003</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>24.099999999999966</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>76.256207355150337</v>
       </c>
-      <c r="G6">
+      <c r="G8">
         <v>43.543430470722079</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="H8">
+        <f>1000-E8-F8-G8</f>
         <v>856.10036217412767</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I8" s="8">
         <v>847.12666666666667</v>
       </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6">
+        <f>I8*J8</f>
         <v>1694.2533333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>29.28</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>70.72</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>0.31824000000000002</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>48.019804714371332</v>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>81.399040373137822</v>
       </c>
-      <c r="G7">
+      <c r="G9">
         <v>34.363842488159179</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
+      <c r="H9">
+        <f>1000-E9-F9-G9</f>
         <v>836.21731242433168</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I9" s="8">
         <v>914.46</v>
       </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7" s="6">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="6">
+        <f>I9*J9</f>
         <v>1828.92</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>34.69</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>65.31</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>0.33308100000000002</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>48.700000000000045</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>79.144507541748013</v>
       </c>
-      <c r="G8">
+      <c r="G10">
         <v>35.582926271907908</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
+      <c r="H10">
+        <f>1000-E10-F10-G10</f>
         <v>836.57256618634403</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I10" s="8">
         <v>803.70666666666659</v>
       </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="1"/>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="6">
+        <f>I10*J10</f>
         <v>1607.4133333333332</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>33.43</v>
+      </c>
+      <c r="C11">
+        <v>66.569999999999993</v>
+      </c>
+      <c r="D11">
+        <v>0.30622199999999999</v>
+      </c>
+      <c r="E11">
+        <v>53.599999999999994</v>
+      </c>
+      <c r="F11">
+        <v>86.740868809939002</v>
+      </c>
+      <c r="G11">
+        <v>30.078812410770652</v>
+      </c>
+      <c r="H11">
+        <f>1000-E11-F11-G11</f>
+        <v>829.58031877929034</v>
+      </c>
+      <c r="I11" s="8">
+        <v>826.35333333333335</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" s="6">
+        <f>I11*J11</f>
+        <v>1652.7066666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>34.53</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>65.47</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>0.25533300000000003</v>
       </c>
-      <c r="E9">
+      <c r="E12">
         <v>35</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>67.443086928142051</v>
       </c>
-      <c r="G9">
+      <c r="G12">
         <v>31.823186344849489</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
+      <c r="H12">
+        <f>1000-E12-F12-G12</f>
         <v>865.73372672700839</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I12" s="8">
         <v>1132.6600000000001</v>
       </c>
-      <c r="J9">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="K9" s="6">
-        <f t="shared" si="1"/>
+      <c r="K12" s="6">
+        <f>I12*J12</f>
         <v>1132.6600000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>94.02</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>5.980000000000004</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <v>7.8936000000000062E-2</v>
       </c>
-      <c r="E10">
+      <c r="E13">
         <v>37.69999999999996</v>
       </c>
-      <c r="F10">
+      <c r="F13">
         <v>71.566937390872738</v>
       </c>
-      <c r="G10">
+      <c r="G13">
         <v>30.533320684066297</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
+      <c r="H13">
+        <f>1000-E13-F13-G13</f>
         <v>860.19974192506095</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>33.82</v>
-      </c>
-      <c r="C11">
-        <v>66.180000000000007</v>
-      </c>
-      <c r="D11">
-        <v>0.26472000000000007</v>
-      </c>
-      <c r="E11">
-        <v>33.499999999999943</v>
-      </c>
-      <c r="F11">
-        <v>66.50553439145925</v>
-      </c>
-      <c r="G11">
-        <v>38.671351790487883</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>861.32311381805289</v>
-      </c>
-      <c r="I11" s="8">
-        <v>1369.7516666666668</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6">
-        <f t="shared" si="1"/>
-        <v>1369.7516666666668</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <v>95.28</v>
-      </c>
-      <c r="C12">
-        <v>4.7199999999999989</v>
-      </c>
-      <c r="D12">
-        <v>5.8999999999999983E-2</v>
-      </c>
-      <c r="E12">
-        <v>35.499999999999972</v>
-      </c>
-      <c r="F12">
-        <v>71.926511192147345</v>
-      </c>
-      <c r="G12">
-        <v>34.250243788566472</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>858.32324501928622</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>33.43</v>
-      </c>
-      <c r="C13">
-        <v>66.569999999999993</v>
-      </c>
-      <c r="D13">
-        <v>0.30622199999999999</v>
-      </c>
-      <c r="E13">
-        <v>53.599999999999994</v>
-      </c>
-      <c r="F13">
-        <v>86.740868809939002</v>
-      </c>
-      <c r="G13">
-        <v>30.078812410770652</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>829.58031877929034</v>
-      </c>
-      <c r="I13" s="8">
-        <v>826.35333333333335</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13" s="6">
-        <f t="shared" si="1"/>
-        <v>1652.7066666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1254,7 @@
         <v>20.26045367290531</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f>1000-E14-F14-G14</f>
         <v>851.74974160234319</v>
       </c>
       <c r="I14" s="8">
@@ -1140,11 +1264,11 @@
         <v>2</v>
       </c>
       <c r="K14" s="6">
-        <f t="shared" si="1"/>
+        <f>I14*J14</f>
         <v>928.04666666666674</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1167,7 +1291,7 @@
         <v>35.844563783065574</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f>1000-E15-F15-G15</f>
         <v>833.88260998018757</v>
       </c>
       <c r="I15" s="8">
@@ -1177,11 +1301,11 @@
         <v>2</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="1"/>
+        <f>I15*J15</f>
         <v>1093.75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1204,13 +1328,13 @@
         <v>32.45726271520644</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f>1000-E16-F16-G16</f>
         <v>860.15393676720987</v>
       </c>
       <c r="I16" s="3"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1233,13 +1357,13 @@
         <v>119.05326714501943</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f>1000-E17-F17-G17</f>
         <v>391.85637710590487</v>
       </c>
       <c r="I17" s="3"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1262,7 +1386,7 @@
         <v>19.017350834877004</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f>1000-E18-F18-G18</f>
         <v>881.45556952528341</v>
       </c>
       <c r="I18" s="8">
@@ -1277,6 +1401,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K18">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1287,25 +1414,25 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="A1:XFD1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,68 +1467,68 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I2" s="2"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I3" s="2"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I4" s="2"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I5" s="3"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K21" s="6"/>
     </row>
   </sheetData>
@@ -1411,28 +1538,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44FE3F3-766B-4687-A015-764259B8488D}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,583 +1595,566 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
+      <c r="B7">
         <v>22.293924653704291</v>
       </c>
-      <c r="C2">
+      <c r="C7">
         <v>77.706075346295705</v>
       </c>
-      <c r="D2">
+      <c r="D7">
         <v>0.31082430138518286</v>
       </c>
-      <c r="E2">
+      <c r="E7">
         <v>30.765331462723822</v>
       </c>
-      <c r="F2">
+      <c r="F7">
         <v>22.175484115686761</v>
       </c>
-      <c r="G2">
+      <c r="G7">
         <v>8.49107151861228</v>
       </c>
-      <c r="H2">
-        <f>1000-E2-F2-G2</f>
+      <c r="H7">
+        <f>1000-E7-F7-G7</f>
         <v>938.56811290297708</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I7" s="8">
         <v>129.27000000000001</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" s="6">
-        <f>I2*J2</f>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6">
+        <f>I7*J7</f>
         <v>258.54000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
+      <c r="B8">
         <v>21.241430978177203</v>
       </c>
-      <c r="C3">
+      <c r="C8">
         <v>78.758569021822794</v>
       </c>
-      <c r="D3">
+      <c r="D8">
         <v>0.22839985016328609</v>
       </c>
-      <c r="E3">
+      <c r="E8">
         <v>25.920640241795354</v>
       </c>
-      <c r="F3">
+      <c r="F8">
         <v>25.139567836158584</v>
       </c>
-      <c r="G3">
+      <c r="G8">
         <v>20.209196719718562</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H18" si="0">1000-E3-F3-G3</f>
+      <c r="H8">
+        <f t="shared" ref="H8:H23" si="0">1000-E8-F8-G8</f>
         <v>928.73059520232755</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I8" s="9">
+        <v>104.30333333333333</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6">
+        <f>I8*J8</f>
+        <v>208.60666666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B9">
         <v>31.06</v>
       </c>
-      <c r="C4">
+      <c r="C9">
         <v>68.94</v>
       </c>
-      <c r="D4">
+      <c r="D9">
         <v>0.19303200000000001</v>
       </c>
-      <c r="E4">
+      <c r="E9">
         <v>26.899999999999977</v>
       </c>
-      <c r="F4">
+      <c r="F9">
         <v>24.337711396275818</v>
       </c>
-      <c r="G4">
+      <c r="G9">
         <v>19.031104979745834</v>
       </c>
-      <c r="H4">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>929.73118362397838</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I9" s="8">
         <v>110.24</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4:K18" si="1">I4*J4</f>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" ref="K9:K23" si="1">I9*J9</f>
         <v>220.48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
+      <c r="B10">
         <v>29.57</v>
       </c>
-      <c r="C5">
+      <c r="C10">
         <v>70.430000000000007</v>
       </c>
-      <c r="D5">
+      <c r="D10">
         <v>0.14790300000000001</v>
       </c>
-      <c r="E5">
+      <c r="E10">
         <v>22.800000000000011</v>
       </c>
-      <c r="F5">
+      <c r="F10">
         <v>28.602554028455401</v>
       </c>
-      <c r="G5">
+      <c r="G10">
         <v>14.08225609104319</v>
       </c>
-      <c r="H5">
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>934.51518988050145</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I10" s="8">
         <v>109.18</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="6">
         <f t="shared" si="1"/>
         <v>218.36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>28.62</v>
       </c>
-      <c r="C6">
+      <c r="C11">
         <v>71.38</v>
       </c>
-      <c r="D6">
+      <c r="D11">
         <v>0.14989799999999998</v>
       </c>
-      <c r="E6">
+      <c r="E11">
         <v>34.399999999999977</v>
       </c>
-      <c r="F6">
+      <c r="F11">
         <v>27.388426579518232</v>
       </c>
-      <c r="G6">
+      <c r="G11">
         <v>23.057361348999478</v>
       </c>
-      <c r="H6">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>915.15421207148233</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I11" s="8">
         <v>108.41000000000001</v>
       </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" s="6">
         <f t="shared" si="1"/>
         <v>216.82000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>27.3</v>
       </c>
-      <c r="C7">
+      <c r="C12">
         <v>72.7</v>
       </c>
-      <c r="D7">
+      <c r="D12">
         <v>0.22536999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E12">
         <v>31.899999999999977</v>
       </c>
-      <c r="F7">
+      <c r="F12">
         <v>28.181794079261643</v>
       </c>
-      <c r="G7">
+      <c r="G12">
         <v>24.540463066975818</v>
       </c>
-      <c r="H7">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>915.37774285376258</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I12" s="8">
         <v>114.55</v>
       </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="6">
         <f t="shared" si="1"/>
         <v>229.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B8">
+      <c r="B13">
         <v>25.98</v>
       </c>
-      <c r="C8">
+      <c r="C13">
         <v>74.02</v>
       </c>
-      <c r="D8">
+      <c r="D13">
         <v>0.14804</v>
       </c>
-      <c r="E8">
+      <c r="E13">
         <v>29.000000000000057</v>
       </c>
-      <c r="F8">
+      <c r="F13">
         <v>32.260237710150911</v>
       </c>
-      <c r="G8">
+      <c r="G13">
         <v>20.064901672779222</v>
       </c>
-      <c r="H8">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>918.67486061706984</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I13" s="8">
         <v>105.815</v>
       </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" s="6">
         <f t="shared" si="1"/>
         <v>211.63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B9">
+      <c r="B14">
         <v>29.85</v>
       </c>
-      <c r="C9">
+      <c r="C14">
         <v>70.150000000000006</v>
       </c>
-      <c r="D9">
+      <c r="D14">
         <v>0.18239</v>
       </c>
-      <c r="E9">
+      <c r="E14">
         <v>35.100000000000051</v>
       </c>
-      <c r="F9">
+      <c r="F14">
         <v>25.488171138835629</v>
       </c>
-      <c r="G9">
+      <c r="G14">
         <v>17.122382230772711</v>
       </c>
-      <c r="H9">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>922.28944663039169</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I14" s="8">
         <v>85.686666666666653</v>
       </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" s="6">
         <f t="shared" si="1"/>
         <v>171.37333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B10">
+      <c r="B15">
         <v>18.326294167812119</v>
       </c>
-      <c r="C10">
+      <c r="C15">
         <v>81.673705832187878</v>
       </c>
-      <c r="E10">
+      <c r="E15">
         <v>35.702306244742488</v>
       </c>
-      <c r="I10" s="8">
-        <v>111.37333333333333</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10" s="6">
-        <f t="shared" si="1"/>
-        <v>222.74666666666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I15" s="8"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B11">
+      <c r="B16">
         <v>17.757737818186264</v>
       </c>
-      <c r="C11">
+      <c r="C16">
         <v>82.242262181813743</v>
       </c>
-      <c r="E11">
+      <c r="E16">
         <v>30.537195369717836</v>
       </c>
-      <c r="I11" s="8">
-        <v>54.563333333333333</v>
-      </c>
-      <c r="J11">
-        <v>2</v>
-      </c>
-      <c r="K11" s="6">
-        <f t="shared" si="1"/>
-        <v>109.12666666666667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="I16" s="8"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B12">
+      <c r="B17">
         <v>17.191238686740423</v>
       </c>
-      <c r="C12">
+      <c r="C17">
         <v>82.808761313259581</v>
       </c>
-      <c r="E12">
+      <c r="E17">
         <v>43.324497496517154</v>
       </c>
-      <c r="I12" s="8">
-        <v>145.06666666666666</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12" s="6">
-        <f t="shared" si="1"/>
-        <v>290.13333333333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="I17" s="8"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B13">
+      <c r="B18">
         <v>16.616082161695964</v>
       </c>
-      <c r="C13">
+      <c r="C18">
         <v>83.383917838304029</v>
       </c>
-      <c r="E13">
+      <c r="E18">
         <v>41.001555507941845</v>
       </c>
-      <c r="I13" s="8">
-        <v>4695.4433333333327</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6">
-        <f t="shared" si="1"/>
-        <v>4695.4433333333327</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="I18" s="8"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B14">
+      <c r="B19">
         <v>17.60573160693783</v>
       </c>
-      <c r="C14">
+      <c r="C19">
         <v>82.394268393062163</v>
       </c>
-      <c r="E14">
+      <c r="E19">
         <v>43.806921266781274</v>
       </c>
-      <c r="I14" s="8"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I19" s="8"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="B15">
+      <c r="B20">
         <v>15.758443043228628</v>
       </c>
-      <c r="C15">
+      <c r="C20">
         <v>84.241556956771376</v>
       </c>
-      <c r="E15">
+      <c r="E20">
         <v>35.169379114513788</v>
       </c>
-      <c r="I15" s="8">
-        <v>1006.4066666666668</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="6">
-        <f t="shared" si="1"/>
-        <v>1006.4066666666668</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I20" s="8"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B16">
+      <c r="B21">
         <v>94.04</v>
       </c>
-      <c r="C16">
+      <c r="C21">
         <v>5.9599999999999937</v>
       </c>
-      <c r="D16">
+      <c r="D21">
         <v>2.3839999999999976E-2</v>
       </c>
-      <c r="E16">
+      <c r="E21">
         <v>53.100000000000023</v>
       </c>
-      <c r="F16">
+      <c r="F21">
         <v>36.298973732443528</v>
       </c>
-      <c r="G16">
+      <c r="G21">
         <v>12.946294575678447</v>
       </c>
-      <c r="H16">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>897.65473169187806</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="I21" s="2"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>43</v>
       </c>
-      <c r="B17">
+      <c r="B22">
         <v>26.96</v>
       </c>
-      <c r="C17">
+      <c r="C22">
         <v>73.039999999999992</v>
       </c>
-      <c r="D17">
+      <c r="D22">
         <v>0.27024799999999993</v>
       </c>
-      <c r="E17">
+      <c r="E22">
         <v>15</v>
       </c>
-      <c r="F17">
+      <c r="F22">
         <v>22.939735073175903</v>
       </c>
-      <c r="G17">
+      <c r="G22">
         <v>29.021400039113338</v>
       </c>
-      <c r="H17">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>933.0388648877107</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I22" s="8">
         <v>95.38333333333334</v>
       </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17" s="6">
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22" s="6">
         <f t="shared" si="1"/>
         <v>190.76666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B18">
+      <c r="B23">
         <v>90.12</v>
       </c>
-      <c r="C18">
+      <c r="C23">
         <v>9.8799999999999955</v>
       </c>
-      <c r="D18">
+      <c r="D23">
         <v>4.3471999999999983E-2</v>
       </c>
-      <c r="E18">
+      <c r="E23">
         <v>42.5</v>
       </c>
-      <c r="F18">
+      <c r="F23">
         <v>43.769490351454181</v>
       </c>
-      <c r="G18">
+      <c r="G23">
         <v>14.444408548484894</v>
       </c>
-      <c r="H18">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>899.28610110006093</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I23" s="8">
         <v>193.655</v>
       </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23" s="6">
         <f t="shared" si="1"/>
         <v>387.31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B19">
+      <c r="B24">
         <v>93.218775192734768</v>
       </c>
-      <c r="C19">
+      <c r="C24">
         <v>6.7812248072652324</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>2.0343674421795695E-2</v>
       </c>
-      <c r="E19">
+      <c r="E24">
         <v>67.17986969847729</v>
       </c>
-      <c r="F19">
+      <c r="F24">
         <v>42.184487184453459</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="I24" s="8"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B20">
+      <c r="B25">
         <v>91.846565408420446</v>
       </c>
-      <c r="C20">
+      <c r="C25">
         <v>8.1534345915795541</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>2.9352364529686391E-2</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>59.068414349412137</v>
       </c>
-      <c r="F20">
+      <c r="F25">
         <v>26.081037994016008</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="6"/>
+      <c r="I25" s="8"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A20">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A7:A25">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2052,29 +2163,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CEFC0F8-0B1F-48A5-8E73-F17095CDF4F8}">
-  <dimension ref="A1:K21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61C0EB4-7B95-43E7-BCBD-6D0CA867A68C}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2108,338 +2219,49 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B2">
-        <v>8.98</v>
+        <v>9.51</v>
       </c>
       <c r="C2">
-        <v>91.02</v>
+        <v>90.49</v>
       </c>
       <c r="D2">
-        <v>1.601952</v>
+        <v>1.4840359999999999</v>
       </c>
       <c r="E2">
-        <v>225.99999999999994</v>
+        <v>72.800000000000011</v>
       </c>
       <c r="F2">
-        <v>160.78964124542912</v>
+        <v>265.38437454205575</v>
       </c>
       <c r="G2">
-        <v>27.249863197175724</v>
+        <v>21.57639125663934</v>
       </c>
       <c r="H2">
         <f>1000-E2-F2-G2</f>
-        <v>585.96049555739512</v>
-      </c>
-      <c r="I2" s="7">
-        <v>5899.1066666666666</v>
+        <v>640.23923420130495</v>
+      </c>
+      <c r="I2">
+        <v>382.96999999999997</v>
       </c>
       <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
-        <f>I2*J2</f>
-        <v>5899.1066666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
-        <v>8.73</v>
-      </c>
-      <c r="C3">
-        <v>91.27</v>
-      </c>
-      <c r="D3">
-        <v>1.679368</v>
-      </c>
-      <c r="E3">
-        <v>233.9</v>
-      </c>
-      <c r="F3">
-        <v>162.71109574709112</v>
-      </c>
-      <c r="G3">
-        <v>6.8361517218186538</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H9" si="0">1000-E3-F3-G3</f>
-        <v>596.55275253109028</v>
-      </c>
-      <c r="I3" s="7">
-        <v>3387.6220000000003</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K9" si="1">I3*J3</f>
-        <v>3387.6220000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="C4">
-        <v>91.55</v>
-      </c>
-      <c r="D4">
-        <v>1.7028300000000001</v>
-      </c>
-      <c r="E4">
-        <v>223.49999999999994</v>
-      </c>
-      <c r="F4">
-        <v>165.21546375842115</v>
-      </c>
-      <c r="G4">
-        <v>50.657498065759114</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>560.62703817581973</v>
-      </c>
-      <c r="I4" s="7">
-        <v>3562.0440000000003</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" si="1"/>
-        <v>3562.0440000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>9.08</v>
-      </c>
-      <c r="C5">
-        <v>90.92</v>
-      </c>
-      <c r="D5">
-        <v>1.6001920000000001</v>
-      </c>
-      <c r="E5">
-        <v>224.50000000000003</v>
-      </c>
-      <c r="F5">
-        <v>154.79722521154883</v>
-      </c>
-      <c r="G5">
-        <v>39.529887563060257</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>581.17288722539092</v>
-      </c>
-      <c r="I5" s="7">
-        <v>5370.74</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6">
-        <f t="shared" si="1"/>
-        <v>5370.74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
-        <v>7.342086670021402</v>
-      </c>
-      <c r="C6">
-        <v>92.657913329978598</v>
-      </c>
-      <c r="D6">
-        <v>1.2230844559557175</v>
-      </c>
-      <c r="E6">
-        <v>238.9929708175832</v>
-      </c>
-      <c r="F6">
-        <v>159.3718955339788</v>
-      </c>
-      <c r="G6">
-        <v>36.537666658495276</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>565.09746698994275</v>
-      </c>
-      <c r="I6" s="7">
-        <v>7882.666666666667</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6">
-        <f t="shared" si="1"/>
-        <v>7882.666666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
-        <v>8.09</v>
-      </c>
-      <c r="C7">
-        <v>91.91</v>
-      </c>
-      <c r="D7">
-        <v>1.01101</v>
-      </c>
-      <c r="E7">
-        <v>221.1</v>
-      </c>
-      <c r="F7">
-        <v>145.94864404681823</v>
-      </c>
-      <c r="G7">
-        <v>10.776615632840269</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>622.17474032034147</v>
-      </c>
-      <c r="I7" s="7">
-        <v>5675.2833333333328</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="6">
-        <f t="shared" si="1"/>
-        <v>5675.2833333333328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8">
-        <v>7.4230302142060669</v>
-      </c>
-      <c r="C8">
-        <v>92.576969785793935</v>
-      </c>
-      <c r="D8">
-        <v>0.70358497037203394</v>
-      </c>
-      <c r="E8">
-        <v>224.49299415987838</v>
-      </c>
-      <c r="F8">
-        <v>181.24304267566859</v>
-      </c>
-      <c r="G8">
-        <v>34.466844194885333</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>559.79711896956769</v>
-      </c>
-      <c r="I8" s="7">
-        <v>926.46499999999992</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8" s="6">
-        <f t="shared" si="1"/>
-        <v>4632.3249999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9">
-        <v>7.4070962017075503</v>
-      </c>
-      <c r="C9">
-        <v>92.592903798292454</v>
-      </c>
-      <c r="D9">
-        <v>0.75926181114599811</v>
-      </c>
-      <c r="E9">
-        <v>236.66748742916823</v>
-      </c>
-      <c r="F9">
-        <v>186.68522844733729</v>
-      </c>
-      <c r="G9">
-        <v>19.035692787986861</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>557.61159133550768</v>
-      </c>
-      <c r="I9" s="7">
-        <v>1167.4199999999998</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" s="6">
-        <f t="shared" si="1"/>
-        <v>5837.0999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f>J2*I2</f>
+        <v>765.93999999999994</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2447,29 +2269,424 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CEFC0F8-0B1F-48A5-8E73-F17095CDF4F8}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>8.98</v>
+      </c>
+      <c r="C2">
+        <v>91.02</v>
+      </c>
+      <c r="D2">
+        <v>1.601952</v>
+      </c>
+      <c r="E2">
+        <v>225.99999999999994</v>
+      </c>
+      <c r="F2">
+        <v>160.78964124542912</v>
+      </c>
+      <c r="G2">
+        <v>27.249863197175724</v>
+      </c>
+      <c r="H2">
+        <f>1000-E2-F2-G2</f>
+        <v>585.96049555739512</v>
+      </c>
+      <c r="I2" s="7">
+        <v>5899.1066666666666</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <f>I2*J2</f>
+        <v>5899.1066666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>8.73</v>
+      </c>
+      <c r="C3">
+        <v>91.27</v>
+      </c>
+      <c r="D3">
+        <v>1.679368</v>
+      </c>
+      <c r="E3">
+        <v>233.9</v>
+      </c>
+      <c r="F3">
+        <v>162.71109574709112</v>
+      </c>
+      <c r="G3">
+        <v>6.8361517218186538</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">1000-E3-F3-G3</f>
+        <v>596.55275253109028</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3387.6220000000003</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K9" si="1">I3*J3</f>
+        <v>3387.6220000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C4">
+        <v>91.55</v>
+      </c>
+      <c r="D4">
+        <v>1.7028300000000001</v>
+      </c>
+      <c r="E4">
+        <v>223.49999999999994</v>
+      </c>
+      <c r="F4">
+        <v>165.21546375842115</v>
+      </c>
+      <c r="G4">
+        <v>50.657498065759114</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>560.62703817581973</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3562.0440000000003</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="1"/>
+        <v>3562.0440000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>9.08</v>
+      </c>
+      <c r="C5">
+        <v>90.92</v>
+      </c>
+      <c r="D5">
+        <v>1.6001920000000001</v>
+      </c>
+      <c r="E5">
+        <v>224.50000000000003</v>
+      </c>
+      <c r="F5">
+        <v>154.79722521154883</v>
+      </c>
+      <c r="G5">
+        <v>39.529887563060257</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>581.17288722539092</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5370.74</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <f t="shared" si="1"/>
+        <v>5370.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>7.342086670021402</v>
+      </c>
+      <c r="C6">
+        <v>92.657913329978598</v>
+      </c>
+      <c r="D6">
+        <v>1.2230844559557175</v>
+      </c>
+      <c r="E6">
+        <v>238.9929708175832</v>
+      </c>
+      <c r="F6">
+        <v>159.3718955339788</v>
+      </c>
+      <c r="G6">
+        <v>36.537666658495276</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>565.09746698994275</v>
+      </c>
+      <c r="I6" s="7">
+        <v>7882.666666666667</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" si="1"/>
+        <v>7882.666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>8.09</v>
+      </c>
+      <c r="C7">
+        <v>91.91</v>
+      </c>
+      <c r="D7">
+        <v>1.01101</v>
+      </c>
+      <c r="E7">
+        <v>221.1</v>
+      </c>
+      <c r="F7">
+        <v>145.94864404681823</v>
+      </c>
+      <c r="G7">
+        <v>10.776615632840269</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>622.17474032034147</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5675.2833333333328</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="1"/>
+        <v>5675.2833333333328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>7.4230302142060669</v>
+      </c>
+      <c r="C8">
+        <v>92.576969785793935</v>
+      </c>
+      <c r="D8">
+        <v>0.70358497037203394</v>
+      </c>
+      <c r="E8">
+        <v>224.49299415987838</v>
+      </c>
+      <c r="F8">
+        <v>181.24304267566859</v>
+      </c>
+      <c r="G8">
+        <v>34.466844194885333</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>559.79711896956769</v>
+      </c>
+      <c r="I8" s="7">
+        <v>926.46499999999992</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="1"/>
+        <v>4632.3249999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>7.4070962017075503</v>
+      </c>
+      <c r="C9">
+        <v>92.592903798292454</v>
+      </c>
+      <c r="D9">
+        <v>0.75926181114599811</v>
+      </c>
+      <c r="E9">
+        <v>236.66748742916823</v>
+      </c>
+      <c r="F9">
+        <v>186.68522844733729</v>
+      </c>
+      <c r="G9">
+        <v>19.035692787986861</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>557.61159133550768</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1167.4199999999998</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="1"/>
+        <v>5837.0999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97342A7-A4B9-46EA-868E-ACCC899EC131}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2504,7 +2721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -2541,64 +2758,64 @@
         <v>26.28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I3" s="4"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I5" s="4"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K21" s="6"/>
     </row>
   </sheetData>
@@ -2607,30 +2824,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B9048-F1D1-4E12-A756-955018FCA9B1}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2702,7 +2919,7 @@
         <v>3152.4933333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2739,7 +2956,7 @@
         <v>947.20666666666659</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2776,7 +2993,7 @@
         <v>1698.3533333333332</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2813,7 +3030,7 @@
         <v>2005.2133333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2850,7 +3067,7 @@
         <v>397.46000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2871,7 +3088,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2892,40 +3109,40 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" s="6"/>
     </row>
   </sheetData>

</xml_diff>